<commit_message>
update_one_column to language table
</commit_message>
<xml_diff>
--- a/1. Application/2. Specifications/1. Data_Catalogue/Data Catalogue.xlsx
+++ b/1. Application/2. Specifications/1. Data_Catalogue/Data Catalogue.xlsx
@@ -315,6 +315,9 @@
     <t>description</t>
   </si>
   <si>
+    <t>VARCHAR2(250)</t>
+  </si>
+  <si>
     <t>The description of the certification</t>
   </si>
   <si>
@@ -343,9 +346,6 @@
   </si>
   <si>
     <t>website</t>
-  </si>
-  <si>
-    <t>VARCHAR2(250)</t>
   </si>
   <si>
     <t>The werbsite of the institution</t>
@@ -688,7 +688,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -700,6 +700,12 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
@@ -818,19 +824,19 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
@@ -872,7 +878,7 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -1278,7 +1284,7 @@
         <v>16</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>207</v>
@@ -1301,7 +1307,7 @@
         <v>16</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>208</v>
@@ -10677,7 +10683,7 @@
         <v>23</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="31.5">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="32.25">
       <c r="A7" s="6">
         <v>6</v>
       </c>
@@ -11510,10 +11516,10 @@
         <v>95</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="G25" s="8" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H25" s="9" t="s">
         <v>21</v>
@@ -11960,16 +11966,16 @@
         <v>16</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F35" s="7" t="s">
         <v>19</v>
       </c>
       <c r="G35" s="8" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H35" s="9" t="s">
         <v>21</v>
@@ -12005,7 +12011,7 @@
         <v>16</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E36" s="7" t="s">
         <v>25</v>
@@ -12014,7 +12020,7 @@
         <v>53</v>
       </c>
       <c r="G36" s="8" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H36" s="9" t="s">
         <v>21</v>
@@ -12050,7 +12056,7 @@
         <v>16</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E37" s="7" t="s">
         <v>47</v>
@@ -12095,7 +12101,7 @@
         <v>16</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E38" s="7" t="s">
         <v>52</v>
@@ -12140,7 +12146,7 @@
         <v>16</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E39" s="7" t="s">
         <v>57</v>
@@ -12185,7 +12191,7 @@
         <v>16</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E40" s="7" t="s">
         <v>59</v>
@@ -12230,7 +12236,7 @@
         <v>16</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E41" s="7" t="s">
         <v>61</v>
@@ -12277,7 +12283,7 @@
         <v>16</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E42" s="7" t="s">
         <v>66</v>
@@ -12324,7 +12330,7 @@
         <v>16</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E43" s="7" t="s">
         <v>70</v>
@@ -12369,7 +12375,7 @@
         <v>16</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E44" s="7" t="s">
         <v>73</v>
@@ -12414,7 +12420,7 @@
         <v>16</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E45" s="7" t="s">
         <v>75</v>
@@ -12461,16 +12467,16 @@
         <v>16</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F46" s="7" t="s">
         <v>19</v>
       </c>
       <c r="G46" s="8" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H46" s="9" t="s">
         <v>21</v>
@@ -12506,7 +12512,7 @@
         <v>16</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E47" s="7" t="s">
         <v>25</v>
@@ -12515,7 +12521,7 @@
         <v>82</v>
       </c>
       <c r="G47" s="8" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H47" s="9" t="s">
         <v>21</v>
@@ -12551,13 +12557,13 @@
         <v>16</v>
       </c>
       <c r="D48" s="7" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="G48" s="8" t="s">
         <v>107</v>
@@ -12596,7 +12602,7 @@
         <v>16</v>
       </c>
       <c r="D49" s="7" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E49" s="7" t="s">
         <v>108</v>
@@ -12641,7 +12647,7 @@
         <v>16</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E50" s="7" t="s">
         <v>43</v>
@@ -12686,7 +12692,7 @@
         <v>16</v>
       </c>
       <c r="D51" s="7" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E51" s="7" t="s">
         <v>95</v>
@@ -12731,7 +12737,7 @@
         <v>16</v>
       </c>
       <c r="D52" s="7" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E52" s="7" t="s">
         <v>47</v>
@@ -12776,7 +12782,7 @@
         <v>16</v>
       </c>
       <c r="D53" s="7" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E53" s="7" t="s">
         <v>52</v>
@@ -12821,7 +12827,7 @@
         <v>16</v>
       </c>
       <c r="D54" s="7" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E54" s="7" t="s">
         <v>57</v>
@@ -12866,7 +12872,7 @@
         <v>16</v>
       </c>
       <c r="D55" s="7" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E55" s="7" t="s">
         <v>59</v>
@@ -12911,7 +12917,7 @@
         <v>16</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E56" s="7" t="s">
         <v>61</v>
@@ -12958,7 +12964,7 @@
         <v>16</v>
       </c>
       <c r="D57" s="7" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E57" s="7" t="s">
         <v>66</v>
@@ -13005,7 +13011,7 @@
         <v>16</v>
       </c>
       <c r="D58" s="7" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E58" s="7" t="s">
         <v>70</v>
@@ -13050,7 +13056,7 @@
         <v>16</v>
       </c>
       <c r="D59" s="7" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E59" s="7" t="s">
         <v>73</v>
@@ -13095,7 +13101,7 @@
         <v>16</v>
       </c>
       <c r="D60" s="7" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E60" s="7" t="s">
         <v>75</v>
@@ -13235,7 +13241,7 @@
         <v>115</v>
       </c>
       <c r="E63" s="7" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F63" s="7" t="s">
         <v>19</v>
@@ -15142,7 +15148,7 @@
         <v>175</v>
       </c>
       <c r="F105" s="7" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="G105" s="8" t="s">
         <v>176</v>
@@ -15912,7 +15918,7 @@
         <v>194</v>
       </c>
       <c r="E122" s="7" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F122" s="7" t="s">
         <v>19</v>

</xml_diff>